<commit_message>
Advances with the report
</commit_message>
<xml_diff>
--- a/reports/figures/All_Models_expanding.xlsx
+++ b/reports/figures/All_Models_expanding.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>config</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>mse_oos</t>
   </si>
@@ -45,110 +42,31 @@
     <t>start_idx</t>
   </si>
   <si>
-    <t>{'name': 'const', 'cv': &lt;class 'src.transform_cv.DisabledCV'&gt;, 'pipeline': Pipeline(memory=None,
-         steps=[('const', ToConstantTransformer()),
-                ('ols',
-                 LinearRegression(copy_X=True, fit_intercept=True, n_jobs=None,
-                                  normalize=False))],
-         verbose=False), 'param_grid': {'ols__fit_intercept': [False]}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
-  </si>
-  <si>
     <t>const</t>
   </si>
   <si>
-    <t>{'name': 'ols', 'cv': &lt;class 'transform_cv.DisabledCV'&gt;, 'pipeline': Pipeline(memory=None,_x000D_
-         steps=[('ols',_x000D_
-                 LinearRegression(copy_X=True, fit_intercept=True, n_jobs=None,_x000D_
-                                  normalize=False))],_x000D_
-         verbose=False), 'param_grid': {'ols__fit_intercept': [True]}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
-  </si>
-  <si>
     <t>ols</t>
   </si>
   <si>
-    <t>{'name': 'pca', 'cv': &lt;class 'TimeSeriesSplitMod.TimeSeriesSplitMod'&gt;, 'pipeline': Pipeline(memory=None,_x000D_
-     steps=[('pca', PCA(copy=True, iterated_power='auto', n_components=None, random_state=None,_x000D_
-  svd_solver='auto', tol=0.0, whiten=False)), ('ols', LinearRegression(copy_X=True, fit_intercept=True, n_jobs=None,_x000D_
-         normalize=False))]), 'param_grid': {'pca__n_components': [1, 2, 3, 4, 5]}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
-  </si>
-  <si>
     <t>pca</t>
   </si>
   <si>
-    <t>{'name': 'enet', 'cv': &lt;class 'TimeSeriesSplitMod.TimeSeriesSplitMod'&gt;, 'pipeline': Pipeline(memory=None,_x000D_
-     steps=[('standard', StandardScaler(copy=True, with_mean=True, with_std=True)), ('enet', ElasticNet(alpha=1.0, copy_X=True, fit_intercept=True, l1_ratio=0.5,_x000D_
-      max_iter=1000, normalize=False, positive=False, precompute=False,_x000D_
-      random_state=None, selection='cyclic', tol=0.0001, warm_start=False))]), 'param_grid': {'enet__alpha': [0.1, 0.5, 0.7, 0.9, 0.97, 0.99], 'enet__l1_ratio': [0, 0.25, 0.5, 0.75, 1], 'enet__random_state': [0]}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
-  </si>
-  <si>
     <t>enet</t>
   </si>
   <si>
-    <t>{'name': 'enet_nocv', 'cv': &lt;class 'src.transform_cv.DisabledCV'&gt;, 'pipeline': Pipeline(memory=None,
-         steps=[('standard',
-                 StandardScaler(copy=True, with_mean=True, with_std=True)),
-                ('enet',
-                 ElasticNet(alpha=1.0, copy_X=True, fit_intercept=True,
-                            l1_ratio=0.5, max_iter=1000, normalize=False,
-                            positive=False, precompute=False, random_state=None,
-                            selection='cyclic', tol=0.0001,
-                            warm_start=False))],
-         verbose=False), 'param_grid': {'enet__random_state': [0]}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
-  </si>
-  <si>
     <t>enet_nocv</t>
   </si>
   <si>
-    <t>{'name': 'pca_enet', 'cv': &lt;class 'TimeSeriesSplitMod.TimeSeriesSplitMod'&gt;, 'pipeline': Pipeline(memory=None,_x000D_
-     steps=[('standard', StandardScaler(copy=True, with_mean=True, with_std=True)), ('pca', PCA(copy=True, iterated_power='auto', n_components=None, random_state=None,_x000D_
-  svd_solver='auto', tol=0.0, whiten=False)), ('enet', ElasticNet(alpha=1.0, copy_X=True, fit_intercept=True, l1_ratio=0.5,_x000D_
-      max_iter=1000, normalize=False, positive=False, precompute=False,_x000D_
-      random_state=None, selection='cyclic', tol=0.0001, warm_start=False))]), 'param_grid': {'enet__alpha': [0.1, 0.5, 0.7, 0.9, 0.97, 0.99], 'enet__l1_ratio': [0, 0.25, 0.5, 0.75, 1], 'enet__random_state': [0]}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
-  </si>
-  <si>
     <t>pca_enet</t>
   </si>
   <si>
-    <t>{'name': 'adab', 'cv': &lt;class 'TimeSeriesSplitMod.TimeSeriesSplitMod'&gt;, 'pipeline': Pipeline(memory=None,_x000D_
-     steps=[('adab', AdaBoostRegressor(base_estimator=None, learning_rate=1.0, loss='linear',_x000D_
-         n_estimators=50, random_state=None))]), 'param_grid': {'adab__random_state': [0], 'adab__n_estimators': [100]}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
-  </si>
-  <si>
     <t>adab</t>
   </si>
   <si>
-    <t>{'name': 'gbr', 'cv': &lt;class 'TimeSeriesSplitMod.TimeSeriesSplitMod'&gt;, 'pipeline': Pipeline(memory=None,_x000D_
-     steps=[('gbr', GradientBoostingRegressor(alpha=0.9, criterion='friedman_mse', init=None,_x000D_
-             learning_rate=0.1, loss='ls', max_depth=3, max_features=None,_x000D_
-             max_leaf_nodes=None, min_impurity_decrease=0.0,_x000D_
-             min_impurity_split=None, min_samples_leaf=1,_x000D_
-             min_...one, subsample=1.0, tol=0.0001,_x000D_
-             validation_fraction=0.1, verbose=0, warm_start=False))]), 'param_grid': {'gbr__random_state': [0], 'gbr__n_estimators': [25, 100, 200], 'gbr__max_depth': [3, 5, 10], 'gbr__learning_rate': [0.05, 0.1, 0.2]}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
-  </si>
-  <si>
     <t>gbr</t>
   </si>
   <si>
-    <t>{'name': 'rf', 'cv': &lt;class 'TimeSeriesSplitMod.TimeSeriesSplitMod'&gt;, 'pipeline': Pipeline(memory=None,_x000D_
-     steps=[('rf', RandomForestRegressor(bootstrap=True, criterion='mse', max_depth=None,_x000D_
-           max_features='auto', max_leaf_nodes=None,_x000D_
-           min_impurity_decrease=0.0, min_impurity_split=None,_x000D_
-           min_samples_leaf=1, min_samples_split=2,_x000D_
-           min_weight_fraction_leaf=0.0, n_estimators='warn', n_jobs=None,_x000D_
-           oob_score=False, random_state=None, verbose=0, warm_start=False))]), 'param_grid': {'rf__random_state': [0], 'rf__n_estimators': [25, 100], 'rf__max_depth': [5, 20], 'rf__min_samples_leaf': [1, 3], 'rf__max_features': [9, 'sqrt']}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
-  </si>
-  <si>
     <t>rf</t>
-  </si>
-  <si>
-    <t>{'name': 'xgb', 'cv': &lt;class 'TimeSeriesSplitMod.TimeSeriesSplitMod'&gt;, 'pipeline': Pipeline(memory=None,_x000D_
-     steps=[('to_numpy', ToNumpyTransformer()), ('xgb', XGBRegressor(base_score=0.5, booster='gbtree', colsample_bylevel=1,_x000D_
-       colsample_bytree=1, gamma=0, importance_type='gain',_x000D_
-       learning_rate=0.1, max_delta_step=0, max_depth=3,_x000D_
-       min_child_weight=1, missing=None, n_estimators=100, n_jobs=1,_x000D_
-       nthread=None, objective='reg:linear', random_state=0, reg_alpha=0,_x000D_
-       reg_lambda=1, scale_pos_weight=1, seed=None, silent=True,_x000D_
-       subsample=1))]), 'param_grid': {'xgb__random_state': [0], 'xgb__n_estimators': [25, 100], 'xgb__max_depth': [5, 10], 'xgb__eta': [0.05, 0.1], 'xgb__alpha': [1, 0.5], 'xgb__lambda': [0, 0.5]}, 'scorer': make_scorer(mean_squared_error, greater_is_better=False), 'grid_search': &lt;class 'sklearn.model_selection._search.GridSearchCV'&gt;}</t>
   </si>
   <si>
     <t>xgb</t>
@@ -635,11 +553,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -961,18 +876,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -980,311 +895,245 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="B2">
+        <v>20.2192097852015</v>
+      </c>
+      <c r="C2">
+        <v>15.942982923399301</v>
+      </c>
+      <c r="D2">
         <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>20.2192097852015</v>
-      </c>
-      <c r="D2">
-        <v>15.942982923399301</v>
       </c>
       <c r="E2">
         <v>0.144611170419295</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
+      <c r="F2">
+        <v>1951</v>
       </c>
       <c r="G2">
-        <v>1951</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>22.534246646317801</v>
       </c>
       <c r="C3">
-        <v>22.534246646317801</v>
+        <v>14.0244030729604</v>
       </c>
       <c r="D3">
-        <v>14.0244030729604</v>
+        <v>-0.114496901002065</v>
       </c>
       <c r="E3">
         <v>1.4080955826521799</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
+      <c r="F3">
+        <v>1951</v>
       </c>
       <c r="G3">
-        <v>1951</v>
-      </c>
-      <c r="H3">
-        <v>-0.114496901002065</v>
-      </c>
-      <c r="I3">
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>20.620293613583002</v>
       </c>
       <c r="C4">
-        <v>20.620293613583002</v>
+        <v>18.1451288215017</v>
       </c>
       <c r="D4">
-        <v>18.1451288215017</v>
+        <v>-1.98367707067863E-2</v>
       </c>
       <c r="E4">
         <v>2.2446320584941302</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
+      <c r="F4">
+        <v>1951</v>
       </c>
       <c r="G4">
-        <v>1951</v>
-      </c>
-      <c r="H4">
-        <v>-1.98367707067863E-2</v>
-      </c>
-      <c r="I4">
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>19.889091062777801</v>
       </c>
       <c r="C5">
-        <v>19.889091062777801</v>
+        <v>17.611954331033399</v>
       </c>
       <c r="D5">
-        <v>17.611954331033399</v>
+        <v>1.6326984384193201E-2</v>
       </c>
       <c r="E5">
         <v>2.90831721239093</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
+      <c r="F5">
+        <v>1951</v>
       </c>
       <c r="G5">
-        <v>1951</v>
-      </c>
-      <c r="H5">
-        <v>1.6326984384193201E-2</v>
-      </c>
-      <c r="I5">
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>20.110843390666101</v>
       </c>
       <c r="C6">
-        <v>20.110843390666101</v>
+        <v>15.7344226804824</v>
       </c>
       <c r="D6">
-        <v>15.7344226804824</v>
+        <v>5.3595761499434201E-3</v>
       </c>
       <c r="E6">
         <v>1.2795359788670799</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
+      <c r="F6">
+        <v>1951</v>
       </c>
       <c r="G6">
-        <v>1951</v>
-      </c>
-      <c r="H6">
-        <v>5.3595761499434201E-3</v>
-      </c>
-      <c r="I6">
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>20.065563238309199</v>
       </c>
       <c r="C7">
-        <v>20.065563238309199</v>
+        <v>17.587134793393702</v>
       </c>
       <c r="D7">
-        <v>17.587134793393702</v>
+        <v>7.59903816838525E-3</v>
       </c>
       <c r="E7">
         <v>2.4269191883143599</v>
       </c>
-      <c r="F7" t="s">
-        <v>19</v>
+      <c r="F7">
+        <v>1951</v>
       </c>
       <c r="G7">
-        <v>1951</v>
-      </c>
-      <c r="H7">
-        <v>7.59903816838525E-3</v>
-      </c>
-      <c r="I7">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>22.080391662720601</v>
       </c>
       <c r="C8">
-        <v>22.080391662720601</v>
+        <v>20.3764610507029</v>
       </c>
       <c r="D8">
-        <v>20.3764610507029</v>
+        <v>-9.2050178878962496E-2</v>
       </c>
       <c r="E8">
         <v>1.0955002314776201</v>
       </c>
-      <c r="F8" t="s">
-        <v>21</v>
+      <c r="F8">
+        <v>1951</v>
       </c>
       <c r="G8">
-        <v>1951</v>
-      </c>
-      <c r="H8">
-        <v>-9.2050178878962496E-2</v>
-      </c>
-      <c r="I8">
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>22.0670295770671</v>
       </c>
       <c r="C9">
-        <v>22.0670295770671</v>
+        <v>19.6621521505595</v>
       </c>
       <c r="D9">
-        <v>19.6621521505595</v>
+        <v>-9.1389317955339694E-2</v>
       </c>
       <c r="E9">
         <v>0.76606355064655896</v>
       </c>
-      <c r="F9" t="s">
-        <v>23</v>
+      <c r="F9">
+        <v>1951</v>
       </c>
       <c r="G9">
-        <v>1951</v>
-      </c>
-      <c r="H9">
-        <v>-9.1389317955339694E-2</v>
-      </c>
-      <c r="I9">
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>20.739690396406399</v>
       </c>
       <c r="C10">
-        <v>20.739690396406399</v>
+        <v>18.495464432489602</v>
       </c>
       <c r="D10">
-        <v>18.495464432489602</v>
+        <v>-2.5741886885501001E-2</v>
       </c>
       <c r="E10">
         <v>1.62379859669412</v>
       </c>
-      <c r="F10" t="s">
-        <v>25</v>
+      <c r="F10">
+        <v>1951</v>
       </c>
       <c r="G10">
-        <v>1951</v>
-      </c>
-      <c r="H10">
-        <v>-2.5741886885501001E-2</v>
-      </c>
-      <c r="I10">
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>23.075231378704299</v>
       </c>
       <c r="C11">
-        <v>23.075231378704299</v>
+        <v>20.443298516050401</v>
       </c>
       <c r="D11">
-        <v>20.443298516050401</v>
+        <v>-0.141252879011774</v>
       </c>
       <c r="E11">
         <v>0.79134177560051999</v>
       </c>
-      <c r="F11" t="s">
-        <v>27</v>
+      <c r="F11">
+        <v>1951</v>
       </c>
       <c r="G11">
-        <v>1951</v>
-      </c>
-      <c r="H11">
-        <v>-0.141252879011774</v>
-      </c>
-      <c r="I11">
         <v>180</v>
       </c>
     </row>

</xml_diff>